<commit_message>
Started to implement the page for generating the score template
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>STUDENT NUMBER</t>
   </si>
@@ -36,6 +36,45 @@
   </si>
   <si>
     <t>SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HASSAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLY </t>
+  </si>
+  <si>
+    <t>LYAWILE</t>
+  </si>
+  <si>
+    <t>GEOGRAPHY</t>
+  </si>
+  <si>
+    <t>KHADIJA</t>
+  </si>
+  <si>
+    <t>YUSUPH</t>
+  </si>
+  <si>
+    <t>SAIBU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUSUF </t>
+  </si>
+  <si>
+    <t>HASSAN</t>
+  </si>
+  <si>
+    <t>YAAQUB</t>
+  </si>
+  <si>
+    <t>TWALIB</t>
+  </si>
+  <si>
+    <t>RASHID</t>
+  </si>
+  <si>
+    <t>AMIR</t>
   </si>
 </sst>
 </file>
@@ -374,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -404,6 +443,846 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
The template download is successfully added
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>STUDENT NUMBER</t>
   </si>
@@ -38,6 +38,18 @@
     <t>SCORE</t>
   </si>
   <si>
+    <t xml:space="preserve">YUSUF </t>
+  </si>
+  <si>
+    <t>HASSAN</t>
+  </si>
+  <si>
+    <t>LYAWILE</t>
+  </si>
+  <si>
+    <t>YAAQUB</t>
+  </si>
+  <si>
     <t>TWALIB</t>
   </si>
   <si>
@@ -51,9 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">ALLY </t>
-  </si>
-  <si>
-    <t>LYAWILE</t>
   </si>
   <si>
     <t>KHADIJA</t>
@@ -401,7 +410,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +443,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -449,51 +458,723 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4"/>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
The student subject list is implemented partially, further implementation will be done in next commit
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>STREAM ID</t>
   </si>
@@ -39,6 +39,18 @@
   </si>
   <si>
     <t>SCORE</t>
+  </si>
+  <si>
+    <t>SAIDI</t>
+  </si>
+  <si>
+    <t>SEIF</t>
+  </si>
+  <si>
+    <t>NGONGO</t>
+  </si>
+  <si>
+    <t>SALMA</t>
   </si>
 </sst>
 </file>
@@ -377,7 +389,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,16 +402,14 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
+      <c r="B2"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -420,6 +430,42 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
The student subjects selection is implemented
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>STREAM ID</t>
   </si>
@@ -39,18 +39,6 @@
   </si>
   <si>
     <t>SCORE</t>
-  </si>
-  <si>
-    <t>SAIDI</t>
-  </si>
-  <si>
-    <t>SEIF</t>
-  </si>
-  <si>
-    <t>NGONGO</t>
-  </si>
-  <si>
-    <t>SALMA</t>
   </si>
 </sst>
 </file>
@@ -389,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -402,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -430,42 +418,6 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>